<commit_message>
modify excelize sheet name
</commit_message>
<xml_diff>
--- a/data/sample.xlsx
+++ b/data/sample.xlsx
@@ -8,7 +8,7 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="146" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="sample" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
 </workbook>
@@ -38,7 +38,7 @@
     <t>sample test!</t>
   </si>
   <si>
-    <t>oops2</t>
+    <t>oops</t>
   </si>
 </sst>
 </file>
@@ -148,7 +148,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>

</xml_diff>